<commit_message>
updating the validation sheet with testcase TC_V_05
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/validation_testing.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/validation_testing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -26,9 +25,6 @@
     <t>Test Scenario</t>
   </si>
   <si>
-    <t>Test Data</t>
-  </si>
-  <si>
     <t>Expected result</t>
   </si>
   <si>
@@ -90,14 +86,86 @@
   </si>
   <si>
     <t>Clock is working and time is being updated at LCD</t>
+  </si>
+  <si>
+    <t>test resources</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hardware resource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: the complete hardware circuit.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>human recorses:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> all team memebrs</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_V_05</t>
+  </si>
+  <si>
+    <t>test the case of pressing muliple switches at the same time</t>
+  </si>
+  <si>
+    <t>Run the System</t>
+  </si>
+  <si>
+    <t>differs from time to time depending on the speed of pressing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -160,15 +228,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -183,6 +257,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -244,7 +327,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,10 +359,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,7 +393,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -487,131 +568,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="3" max="4" width="42.5703125" customWidth="1"/>
     <col min="5" max="5" width="46.140625" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="45">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+    <row r="3" spans="1:7" ht="125.25" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="5"/>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="4" spans="1:7" ht="120" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6"/>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
+    <row r="5" spans="1:7" ht="45">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+    <row r="6" spans="1:7" ht="60">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:D6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the resourcs needed for the validation
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/validation_testing.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/validation_testing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>test resources</t>
+  </si>
+  <si>
+    <t>TC_V_05</t>
+  </si>
+  <si>
+    <t>test the case of pressing muliple switches at the same time</t>
+  </si>
+  <si>
+    <t>Run the System</t>
+  </si>
+  <si>
+    <t>differs from time to time depending on the speed of pressing</t>
   </si>
   <si>
     <r>
@@ -111,7 +123,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: the complete hardware circuit.</t>
+      <t>: the complete hardware circuit, oscillscope for measuring the clock width</t>
     </r>
   </si>
   <si>
@@ -125,7 +137,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>human recorses:</t>
+      <t>Software resources:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">application code </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     human recorses:</t>
     </r>
     <r>
       <rPr>
@@ -139,23 +186,20 @@
     </r>
   </si>
   <si>
-    <t>TC_V_05</t>
-  </si>
-  <si>
-    <t>test the case of pressing muliple switches at the same time</t>
-  </si>
-  <si>
-    <t>Run the System</t>
-  </si>
-  <si>
-    <t>differs from time to time depending on the speed of pressing</t>
+    <t>PENDING</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>PASSEd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +210,14 @@
     <font>
       <b/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -205,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -229,8 +281,23 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -241,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,11 +328,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,13 +688,15 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="125.25" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -636,8 +708,8 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>26</v>
+      <c r="D3" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -645,7 +717,9 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="120" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -657,14 +731,18 @@
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="45">
       <c r="A5" s="2" t="s">
@@ -683,30 +761,34 @@
       <c r="F5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="60">
       <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
modifying validation sheet according to the APP_test for the finction getTIme
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/validation_testing.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/validation_testing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -70,9 +70,6 @@
     <t>switch between hours,seconds,minutes,AM/PM using mode switch,press increment or decrement switch for less than 3 seconds then press again for more than 3 seconds</t>
   </si>
   <si>
-    <t>switch between hours,seconds,minutes,AM/PM using mode switch.for example if mode switch was pressed for 1 time and increment switch is pressed for less than 3 seconds minutes will be incremented by 1 but if switch is pressed for more than 3 seconds minutes will keep incrementing till switch is released</t>
-  </si>
-  <si>
     <t>Actual result was as expected</t>
   </si>
   <si>
@@ -89,18 +86,6 @@
   </si>
   <si>
     <t>test resources</t>
-  </si>
-  <si>
-    <t>TC_V_05</t>
-  </si>
-  <si>
-    <t>test the case of pressing muliple switches at the same time</t>
-  </si>
-  <si>
-    <t>Run the System</t>
-  </si>
-  <si>
-    <t>differs from time to time depending on the speed of pressing</t>
   </si>
   <si>
     <r>
@@ -123,7 +108,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: the complete hardware circuit, oscillscope for measuring the clock width</t>
+      <t>: the complete hardware circuit.</t>
     </r>
   </si>
   <si>
@@ -137,42 +122,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Software resources:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">application code </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">     human recorses:</t>
+      <t>human recorses:</t>
     </r>
     <r>
       <rPr>
@@ -186,20 +136,26 @@
     </r>
   </si>
   <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>PASSED</t>
-  </si>
-  <si>
-    <t>PASSEd</t>
+    <t>TC_V_05</t>
+  </si>
+  <si>
+    <t>test the case of pressing muliple switches at the same time</t>
+  </si>
+  <si>
+    <t>Run the System</t>
+  </si>
+  <si>
+    <t>differs from time to time depending on the speed of pressing</t>
+  </si>
+  <si>
+    <t>switch between hours,seconds,minutes,AM/PM using middle switch.for example if middle switch was pressed for 1 time and increment switch is pressed for less than 3 seconds minutes will be incremented by 1 but if switch is pressed for more than 3 seconds minutes will keep incrementing till switch is released</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,14 +166,6 @@
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -257,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -281,23 +229,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -308,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,14 +261,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,7 +327,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -429,9 +359,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -463,6 +394,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -638,14 +570,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -654,7 +586,7 @@
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -677,7 +609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -688,17 +620,15 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="125.25" customHeight="1">
+    <row r="3" spans="1:7" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -708,8 +638,8 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>31</v>
+      <c r="D3" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -717,11 +647,9 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="120" customHeight="1">
+    <row r="4" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -731,64 +659,56 @@
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="60">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D3:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>

</xml_diff>